<commit_message>
Implement auth UX improvements and admin/HEI display updates
</commit_message>
<xml_diff>
--- a/server/data/Form 1.xlsx
+++ b/server/data/Form 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EMMAN\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5333BEA-9CD7-4CE2-ADBF-BC9BFF82B207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CC0ADE-1AD2-4F1A-975C-4B00740C8968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20124" yWindow="3420" windowWidth="17088" windowHeight="12120" xr2:uid="{F0BD72CC-BF34-4528-9B18-D10B09C92EED}"/>
+    <workbookView xWindow="20472" yWindow="3768" windowWidth="17088" windowHeight="12120" xr2:uid="{F0BD72CC-BF34-4528-9B18-D10B09C92EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Name of HEI: ________________________________________________________________________________________</t>
   </si>
@@ -80,10 +80,37 @@
     <t>Bachelor's</t>
   </si>
   <si>
-    <t>A. IP Studies/Education to be offered as an Elective Subject</t>
-  </si>
-  <si>
     <t>Academic Year: __________________________</t>
+  </si>
+  <si>
+    <t>Prepared by:</t>
+  </si>
+  <si>
+    <t>Reviewed by:</t>
+  </si>
+  <si>
+    <t>Approved By:</t>
+  </si>
+  <si>
+    <t>__________________________________</t>
+  </si>
+  <si>
+    <t>______________________________________</t>
+  </si>
+  <si>
+    <t>Name and Signature of Official</t>
+  </si>
+  <si>
+    <t>Dean/Department Head</t>
+  </si>
+  <si>
+    <t>VPAA</t>
+  </si>
+  <si>
+    <t>President</t>
+  </si>
+  <si>
+    <t>B. IP Studies/Education to be offered as an Elective Subject</t>
   </si>
 </sst>
 </file>
@@ -115,7 +142,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -263,47 +290,53 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -322,46 +355,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -701,101 +701,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81285C4A-9BC0-458C-A427-4883E2EF0FAA}">
-  <dimension ref="A3:M29"/>
+  <dimension ref="A3:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="8.88671875" style="3"/>
-    <col min="9" max="9" width="10.109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.77734375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="8" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="10.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="K5" s="28" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="K5" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="10" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="23" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="8" t="s">
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="25" t="s">
+      <c r="I10" s="18"/>
+      <c r="J10" s="22" t="s">
         <v>9</v>
       </c>
       <c r="K10" s="4" t="s">
@@ -805,148 +805,148 @@
       <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="27" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L11" s="27" t="s">
+      <c r="L11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M11" s="27" t="s">
+      <c r="M11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="27"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="4"/>
       <c r="F12" s="5"/>
       <c r="G12" s="6"/>
       <c r="H12" s="4"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
+      <c r="D13" s="2"/>
       <c r="E13" s="4"/>
       <c r="F13" s="5"/>
       <c r="G13" s="6"/>
       <c r="H13" s="4"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
+      <c r="D14" s="2"/>
       <c r="E14" s="4"/>
       <c r="F14" s="5"/>
       <c r="G14" s="6"/>
       <c r="H14" s="4"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
+      <c r="D15" s="2"/>
       <c r="E15" s="4"/>
       <c r="F15" s="5"/>
       <c r="G15" s="6"/>
       <c r="H15" s="4"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
+      <c r="D16" s="2"/>
       <c r="E16" s="4"/>
       <c r="F16" s="5"/>
       <c r="G16" s="6"/>
       <c r="H16" s="4"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
+      <c r="D17" s="2"/>
       <c r="E17" s="4"/>
       <c r="F17" s="5"/>
       <c r="G17" s="6"/>
       <c r="H17" s="4"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+      <c r="A20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="22" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="23" t="s">
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="8" t="s">
+      <c r="F22" s="17"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="I22" s="10"/>
-      <c r="J22" s="25" t="s">
+      <c r="I22" s="18"/>
+      <c r="J22" s="22" t="s">
         <v>9</v>
       </c>
       <c r="K22" s="4" t="s">
@@ -956,164 +956,198 @@
       <c r="M22" s="6"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="27" t="s">
+      <c r="A23" s="11"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L23" s="27" t="s">
+      <c r="L23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M23" s="27" t="s">
+      <c r="M23" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="27"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="3"/>
       <c r="E24" s="4"/>
       <c r="F24" s="5"/>
       <c r="G24" s="6"/>
       <c r="H24" s="4"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="7"/>
+      <c r="D25" s="2"/>
       <c r="E25" s="4"/>
       <c r="F25" s="5"/>
       <c r="G25" s="6"/>
       <c r="H25" s="4"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="7"/>
+      <c r="D26" s="2"/>
       <c r="E26" s="4"/>
       <c r="F26" s="5"/>
       <c r="G26" s="6"/>
       <c r="H26" s="4"/>
       <c r="I26" s="6"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
-      <c r="D27" s="7"/>
+      <c r="D27" s="2"/>
       <c r="E27" s="4"/>
       <c r="F27" s="5"/>
       <c r="G27" s="6"/>
       <c r="H27" s="4"/>
       <c r="I27" s="6"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
-      <c r="D28" s="7"/>
+      <c r="D28" s="2"/>
       <c r="E28" s="4"/>
       <c r="F28" s="5"/>
       <c r="G28" s="6"/>
       <c r="H28" s="4"/>
       <c r="I28" s="6"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
-      <c r="D29" s="7"/>
+      <c r="D29" s="2"/>
       <c r="E29" s="4"/>
       <c r="F29" s="5"/>
       <c r="G29" s="6"/>
       <c r="H29" s="4"/>
       <c r="I29" s="6"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="E33" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="K33" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="E36" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="K36" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="E37" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="K37" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="E38" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="K38" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="53">
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="A20:I20"/>
-    <mergeCell ref="A22:C24"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:G23"/>
-    <mergeCell ref="H22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A10:C12"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:G11"/>
-    <mergeCell ref="H10:I11"/>
-    <mergeCell ref="J10:J11"/>
+  <mergeCells count="67">
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="K36:M36"/>
     <mergeCell ref="K10:M10"/>
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="A6:I6"/>
@@ -1121,6 +1155,54 @@
     <mergeCell ref="D3:J3"/>
     <mergeCell ref="K5:M5"/>
     <mergeCell ref="J6:M6"/>
+    <mergeCell ref="A10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:G11"/>
+    <mergeCell ref="H10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:G23"/>
+    <mergeCell ref="H22:I23"/>
+    <mergeCell ref="A22:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:I29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>